<commit_message>
hiển thị popup tính cước ô tô
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/cuocoto/theotongculy.xlsx
+++ b/Worksheet/Content/Template/cuocoto/theotongculy.xlsx
@@ -485,14 +485,14 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -795,7 +795,7 @@
   <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection sqref="A1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -829,197 +829,197 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="R1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="U1" s="57" t="s">
+      <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="58" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="58" t="s">
+      <c r="A2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="59" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="S3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="U3" s="58" t="s">
+      <c r="A3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="59" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1052,72 +1052,72 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="57" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59" t="s">
+      <c r="J7" s="57"/>
+      <c r="K7" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59" t="s">
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59" t="s">
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59" t="s">
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="59" t="s">
+      <c r="U7" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="59"/>
-      <c r="W7" s="59" t="s">
+      <c r="V7" s="57"/>
+      <c r="W7" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="X7" s="59" t="s">
+      <c r="X7" s="57" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="60"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
       <c r="I8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1151,15 +1151,15 @@
       <c r="S8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="T8" s="59"/>
+      <c r="T8" s="57"/>
       <c r="U8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="W8" s="59"/>
-      <c r="X8" s="59"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -1595,14 +1595,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A2:U2"/>
     <mergeCell ref="A3:U3"/>
@@ -1614,6 +1606,14 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="T7:T8"/>
     <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
   </mergeCells>
   <conditionalFormatting sqref="J9:J14">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
@@ -1666,207 +1666,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="L1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="O1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="57" t="s">
+      <c r="T1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="57" t="s">
+      <c r="U1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="57" t="s">
+      <c r="V1" s="58" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="58" t="s">
+      <c r="A2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="59" t="s">
         <v>1</v>
       </c>
       <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="S3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="U3" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="V3" s="58" t="s">
+      <c r="A3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="59" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1880,61 +1880,61 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59" t="s">
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-      <c r="T5" s="59" t="s">
+      <c r="T5" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="U5" s="59" t="s">
+      <c r="U5" s="57" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="60"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
       <c r="I6" s="7" t="s">
         <v>56</v>
       </c>
@@ -1968,8 +1968,8 @@
       <c r="S6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>

</xml_diff>